<commit_message>
chore: partial 3.3.0 results
</commit_message>
<xml_diff>
--- a/load-testing/server/results.xlsx
+++ b/load-testing/server/results.xlsx
@@ -22,7 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
   <si>
-    <t xml:space="preserve">Sequetial Ingest Speed Test</t>
+    <t xml:space="preserve">Sequential Ingest Speed Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
   </si>
   <si>
     <t xml:space="preserve">Run 1</t>
@@ -44,15 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">Run 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average</t>
   </si>
   <si>
     <t xml:space="preserve">1 pipeline</t>
@@ -119,6 +119,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,6 +141,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,11 +195,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,10 +231,10 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
   </cols>
@@ -251,16 +253,16 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -277,114 +279,114 @@
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
+        <f aca="false">MIN(F2:L2)</f>
         <v>700</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
+        <f aca="false">MAX(F2:L2)</f>
+        <v>757</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <f aca="false">AVERAGE(F2:L2)</f>
+        <v>733.142857142857</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>744</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>746</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>757</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>741</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>740</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>704</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <f aca="false">MIN(C2:I2)</f>
-        <v>700</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <f aca="false">MAX(C2:I2)</f>
-        <v>757</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <f aca="false">AVERAGE(C2:I2)</f>
-        <v>733.142857142857</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
+        <f aca="false">MIN(F3:L3)</f>
+        <v>1222</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">MAX(F3:L3)</f>
+        <v>1329</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <f aca="false">AVERAGE(F3:L3)</f>
+        <v>1281.14285714286</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>1234</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>1222</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>1293</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>1319</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>1278</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>1329</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>1293</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <f aca="false">MIN(C3:I3)</f>
-        <v>1222</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <f aca="false">MAX(C3:I3)</f>
-        <v>1329</v>
-      </c>
-      <c r="L3" s="4" t="n">
-        <f aca="false">AVERAGE(C3:I3)</f>
-        <v>1281.14285714286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
+        <f aca="false">MIN(F4:L4)</f>
+        <v>1636</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">MAX(F4:L4)</f>
+        <v>1745</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <f aca="false">AVERAGE(F4:L4)</f>
+        <v>1700.71428571429</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>1712</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>1745</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>1739</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>1636</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>1675</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>1729</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>1669</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <f aca="false">MIN(C4:I4)</f>
-        <v>1636</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <f aca="false">MAX(C4:I4)</f>
-        <v>1745</v>
-      </c>
-      <c r="L4" s="4" t="n">
-        <f aca="false">AVERAGE(C4:I4)</f>
-        <v>1700.71428571429</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,16 +403,16 @@
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="3" t="s">
@@ -427,87 +429,87 @@
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
+        <f aca="false">MIN(F7:L7)</f>
+        <v>943</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">MAX(F7:L7)</f>
         <v>970</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="4" t="n">
+        <f aca="false">AVERAGE(F7:L7)</f>
+        <v>956.5</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>970</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="G7" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>943</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>943</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <f aca="false">MIN(C7:I7)</f>
-        <v>943</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <f aca="false">MAX(C7:I7)</f>
-        <v>970</v>
-      </c>
-      <c r="L7" s="4" t="n">
-        <f aca="false">AVERAGE(C7:I7)</f>
-        <v>956.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
+        <f aca="false">MIN(F8:L8)</f>
+        <v>602</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">MAX(F8:L8)</f>
+        <v>996</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <f aca="false">AVERAGE(F8:L8)</f>
+        <v>740.25</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>612</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>602</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>996</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>751</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <f aca="false">MIN(C8:I8)</f>
-        <v>602</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <f aca="false">MAX(C8:I8)</f>
-        <v>996</v>
-      </c>
-      <c r="L8" s="4" t="n">
-        <f aca="false">AVERAGE(C8:I8)</f>
-        <v>740.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
+        <f aca="false">MIN(F9:L9)</f>
+        <v>331</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">MAX(F9:L9)</f>
+        <v>646</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <f aca="false">AVERAGE(F9:L9)</f>
+        <v>502.25</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>559</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>473</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>331</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>646</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <f aca="false">MIN(C9:I9)</f>
-        <v>331</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <f aca="false">MAX(C9:I9)</f>
-        <v>646</v>
-      </c>
-      <c r="L9" s="4" t="n">
-        <f aca="false">AVERAGE(C9:I9)</f>
-        <v>502.25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,16 +526,16 @@
       <c r="E11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -553,16 +555,16 @@
       <c r="B12" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="1" t="n">
-        <f aca="false">MIN(C12:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="n">
-        <f aca="false">MAX(C12:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="4" t="e">
-        <f aca="false">AVERAGE(C12:I12)</f>
+      <c r="C12" s="1" t="n">
+        <f aca="false">MIN(F12:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">MAX(F12:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="e">
+        <f aca="false">AVERAGE(F12:L12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -573,16 +575,16 @@
       <c r="B13" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="1" t="n">
-        <f aca="false">MIN(C13:I13)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <f aca="false">MAX(C13:I13)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="4" t="e">
-        <f aca="false">AVERAGE(C13:I13)</f>
+      <c r="C13" s="1" t="n">
+        <f aca="false">MIN(F13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">MAX(F13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="e">
+        <f aca="false">AVERAGE(F13:L13)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -593,16 +595,16 @@
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1" t="n">
-        <f aca="false">MIN(C14:I14)</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="n">
-        <f aca="false">MAX(C14:I14)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="4" t="e">
-        <f aca="false">AVERAGE(C14:I14)</f>
+      <c r="C14" s="1" t="n">
+        <f aca="false">MIN(F14:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">MAX(F14:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="e">
+        <f aca="false">AVERAGE(F14:L14)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -613,16 +615,16 @@
       <c r="B15" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="1" t="n">
-        <f aca="false">MIN(C15:I15)</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <f aca="false">MAX(C15:I15)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="4" t="e">
-        <f aca="false">AVERAGE(C15:I15)</f>
+      <c r="C15" s="1" t="n">
+        <f aca="false">MIN(F15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">MAX(F15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="e">
+        <f aca="false">AVERAGE(F15:L15)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -633,16 +635,16 @@
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="1" t="n">
-        <f aca="false">MIN(C16:I16)</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <f aca="false">MAX(C16:I16)</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="4" t="e">
-        <f aca="false">AVERAGE(C16:I16)</f>
+      <c r="C16" s="1" t="n">
+        <f aca="false">MIN(F16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">MAX(F16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="e">
+        <f aca="false">AVERAGE(F16:L16)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -653,16 +655,16 @@
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="1" t="n">
-        <f aca="false">MIN(C17:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <f aca="false">MAX(C17:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="4" t="e">
-        <f aca="false">AVERAGE(C17:I17)</f>
+      <c r="C17" s="1" t="n">
+        <f aca="false">MIN(F17:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">MAX(F17:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="e">
+        <f aca="false">AVERAGE(F17:L17)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -673,16 +675,16 @@
       <c r="B18" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="1" t="n">
-        <f aca="false">MIN(C18:I18)</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <f aca="false">MAX(C18:I18)</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="4" t="e">
-        <f aca="false">AVERAGE(C18:I18)</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">MIN(F18:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">MAX(F18:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="e">
+        <f aca="false">AVERAGE(F18:L18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -693,16 +695,16 @@
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="1" t="n">
-        <f aca="false">MIN(C19:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <f aca="false">MAX(C19:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="4" t="e">
-        <f aca="false">AVERAGE(C19:I19)</f>
+      <c r="C19" s="1" t="n">
+        <f aca="false">MIN(F19:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">MAX(F19:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="e">
+        <f aca="false">AVERAGE(F19:L19)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -713,16 +715,16 @@
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="1" t="n">
-        <f aca="false">MIN(C20:I20)</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="n">
-        <f aca="false">MAX(C20:I20)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="4" t="e">
-        <f aca="false">AVERAGE(C20:I20)</f>
+      <c r="C20" s="1" t="n">
+        <f aca="false">MIN(F20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">MAX(F20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="e">
+        <f aca="false">AVERAGE(F20:L20)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -740,16 +742,16 @@
       <c r="E22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J22" s="3" t="s">
@@ -769,16 +771,16 @@
       <c r="B23" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="1" t="n">
-        <f aca="false">MIN(C23:I23)</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <f aca="false">MAX(C23:I23)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="4" t="e">
-        <f aca="false">AVERAGE(C23:I23)</f>
+      <c r="C23" s="1" t="n">
+        <f aca="false">MIN(F23:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">MAX(F23:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="e">
+        <f aca="false">AVERAGE(F23:L23)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -789,16 +791,16 @@
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="1" t="n">
-        <f aca="false">MIN(C24:I24)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="1" t="n">
-        <f aca="false">MAX(C24:I24)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="4" t="e">
-        <f aca="false">AVERAGE(C24:I24)</f>
+      <c r="C24" s="1" t="n">
+        <f aca="false">MIN(F24:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">MAX(F24:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="e">
+        <f aca="false">AVERAGE(F24:L24)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -809,16 +811,16 @@
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="1" t="n">
-        <f aca="false">MIN(C25:I25)</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <f aca="false">MAX(C25:I25)</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="4" t="e">
-        <f aca="false">AVERAGE(C25:I25)</f>
+      <c r="C25" s="1" t="n">
+        <f aca="false">MIN(F25:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">MAX(F25:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="e">
+        <f aca="false">AVERAGE(F25:L25)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -829,16 +831,16 @@
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="1" t="n">
-        <f aca="false">MIN(C26:I26)</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <f aca="false">MAX(C26:I26)</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="4" t="e">
-        <f aca="false">AVERAGE(C26:I26)</f>
+      <c r="C26" s="1" t="n">
+        <f aca="false">MIN(F26:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">MAX(F26:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="e">
+        <f aca="false">AVERAGE(F26:L26)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -849,16 +851,16 @@
       <c r="B27" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="1" t="n">
-        <f aca="false">MIN(C27:I27)</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <f aca="false">MAX(C27:I27)</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="4" t="e">
-        <f aca="false">AVERAGE(C27:I27)</f>
+      <c r="C27" s="1" t="n">
+        <f aca="false">MIN(F27:L27)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">MAX(F27:L27)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="e">
+        <f aca="false">AVERAGE(F27:L27)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -869,16 +871,16 @@
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="1" t="n">
-        <f aca="false">MIN(C28:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <f aca="false">MAX(C28:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="4" t="e">
-        <f aca="false">AVERAGE(C28:I28)</f>
+      <c r="C28" s="1" t="n">
+        <f aca="false">MIN(F28:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">MAX(F28:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="e">
+        <f aca="false">AVERAGE(F28:L28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -889,16 +891,16 @@
       <c r="B29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="1" t="n">
-        <f aca="false">MIN(C29:I29)</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="1" t="n">
-        <f aca="false">MAX(C29:I29)</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="4" t="e">
-        <f aca="false">AVERAGE(C29:I29)</f>
+      <c r="C29" s="1" t="n">
+        <f aca="false">MIN(F29:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">MAX(F29:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="e">
+        <f aca="false">AVERAGE(F29:L29)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -909,16 +911,16 @@
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="1" t="n">
-        <f aca="false">MIN(C30:I30)</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <f aca="false">MAX(C30:I30)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="4" t="e">
-        <f aca="false">AVERAGE(C30:I30)</f>
+      <c r="C30" s="1" t="n">
+        <f aca="false">MIN(F30:L30)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">MAX(F30:L30)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="e">
+        <f aca="false">AVERAGE(F30:L30)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -929,16 +931,16 @@
       <c r="B31" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="1" t="n">
-        <f aca="false">MIN(C31:I31)</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="1" t="n">
-        <f aca="false">MAX(C31:I31)</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="4" t="e">
-        <f aca="false">AVERAGE(C31:I31)</f>
+      <c r="C31" s="1" t="n">
+        <f aca="false">MIN(F31:L31)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">MAX(F31:L31)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="e">
+        <f aca="false">AVERAGE(F31:L31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -955,16 +957,16 @@
       <c r="E33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J33" s="3" t="s">
@@ -981,16 +983,16 @@
       <c r="A34" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="1" t="n">
-        <f aca="false">MIN(C34:I34)</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="1" t="n">
-        <f aca="false">MAX(C34:I34)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="4" t="e">
-        <f aca="false">AVERAGE(C34:I34)</f>
+      <c r="C34" s="1" t="n">
+        <f aca="false">MIN(F34:L34)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">MAX(F34:L34)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="e">
+        <f aca="false">AVERAGE(F34:L34)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -998,16 +1000,16 @@
       <c r="A35" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="J35" s="1" t="n">
-        <f aca="false">MIN(C35:I35)</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="1" t="n">
-        <f aca="false">MAX(C35:I35)</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="4" t="e">
-        <f aca="false">AVERAGE(C35:I35)</f>
+      <c r="C35" s="1" t="n">
+        <f aca="false">MIN(F35:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">MAX(F35:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="e">
+        <f aca="false">AVERAGE(F35:L35)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1015,16 +1017,16 @@
       <c r="A36" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="1" t="n">
-        <f aca="false">MIN(C36:I36)</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="1" t="n">
-        <f aca="false">MAX(C36:I36)</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="4" t="e">
-        <f aca="false">AVERAGE(C36:I36)</f>
+      <c r="C36" s="1" t="n">
+        <f aca="false">MIN(F36:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">MAX(F36:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="e">
+        <f aca="false">AVERAGE(F36:L36)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1032,16 +1034,16 @@
       <c r="A37" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="1" t="n">
-        <f aca="false">MIN(C37:I37)</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="1" t="n">
-        <f aca="false">MAX(C37:I37)</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="4" t="e">
-        <f aca="false">AVERAGE(C37:I37)</f>
+      <c r="C37" s="1" t="n">
+        <f aca="false">MIN(F37:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">MAX(F37:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="e">
+        <f aca="false">AVERAGE(F37:L37)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1049,16 +1051,16 @@
       <c r="A38" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="1" t="n">
-        <f aca="false">MIN(C38:I38)</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="1" t="n">
-        <f aca="false">MAX(C38:I38)</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="4" t="e">
-        <f aca="false">AVERAGE(C38:I38)</f>
+      <c r="C38" s="1" t="n">
+        <f aca="false">MIN(F38:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">MAX(F38:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="e">
+        <f aca="false">AVERAGE(F38:L38)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1066,16 +1068,16 @@
       <c r="A39" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="J39" s="1" t="n">
-        <f aca="false">MIN(C39:I39)</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="n">
-        <f aca="false">MAX(C39:I39)</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="4" t="e">
-        <f aca="false">AVERAGE(C39:I39)</f>
+      <c r="C39" s="1" t="n">
+        <f aca="false">MIN(F39:L39)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">MAX(F39:L39)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="e">
+        <f aca="false">AVERAGE(F39:L39)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1083,16 +1085,16 @@
       <c r="A40" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="1" t="n">
-        <f aca="false">MIN(C40:I40)</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="1" t="n">
-        <f aca="false">MAX(C40:I40)</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="4" t="e">
-        <f aca="false">AVERAGE(C40:I40)</f>
+      <c r="C40" s="1" t="n">
+        <f aca="false">MIN(F40:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">MAX(F40:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="e">
+        <f aca="false">AVERAGE(F40:L40)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1100,16 +1102,16 @@
       <c r="A41" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J41" s="1" t="n">
-        <f aca="false">MIN(C41:I41)</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="1" t="n">
-        <f aca="false">MAX(C41:I41)</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="4" t="e">
-        <f aca="false">AVERAGE(C41:I41)</f>
+      <c r="C41" s="1" t="n">
+        <f aca="false">MIN(F41:L41)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">MAX(F41:L41)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="e">
+        <f aca="false">AVERAGE(F41:L41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: add 3.4.0 worksheet
</commit_message>
<xml_diff>
--- a/load-testing/server/results.xlsx
+++ b/load-testing/server/results.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server 3.3.0" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Server 3.4.0" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="28">
   <si>
     <t xml:space="preserve">Sequential Ingest Speed Test</t>
   </si>
@@ -230,11 +231,11 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
   </cols>
@@ -1124,4 +1125,808 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">MIN(F2:L2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">MAX(F2:L2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="e">
+        <f aca="false">AVERAGE(F2:L2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">MIN(F3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">MAX(F3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="e">
+        <f aca="false">AVERAGE(F3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">MIN(F4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">MAX(F4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="e">
+        <f aca="false">AVERAGE(F4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <f aca="false">MIN(F7:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">MAX(F7:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="e">
+        <f aca="false">AVERAGE(F7:L7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="false">MIN(F8:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">MAX(F8:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="e">
+        <f aca="false">AVERAGE(F8:L8)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="false">MIN(F9:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">MAX(F9:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="e">
+        <f aca="false">AVERAGE(F9:L9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="false">MIN(F12:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">MAX(F12:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="e">
+        <f aca="false">AVERAGE(F12:L12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="false">MIN(F13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">MAX(F13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="e">
+        <f aca="false">AVERAGE(F13:L13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <f aca="false">MIN(F14:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">MAX(F14:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="e">
+        <f aca="false">AVERAGE(F14:L14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <f aca="false">MIN(F15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">MAX(F15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="e">
+        <f aca="false">AVERAGE(F15:L15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <f aca="false">MIN(F16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">MAX(F16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="e">
+        <f aca="false">AVERAGE(F16:L16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">MIN(F17:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">MAX(F17:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="e">
+        <f aca="false">AVERAGE(F17:L17)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">MIN(F18:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">MAX(F18:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="e">
+        <f aca="false">AVERAGE(F18:L18)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">MIN(F19:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">MAX(F19:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="e">
+        <f aca="false">AVERAGE(F19:L19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="false">MIN(F20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">MAX(F20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="e">
+        <f aca="false">AVERAGE(F20:L20)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">MIN(F23:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">MAX(F23:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="e">
+        <f aca="false">AVERAGE(F23:L23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">MIN(F24:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">MAX(F24:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="e">
+        <f aca="false">AVERAGE(F24:L24)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">MIN(F25:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">MAX(F25:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="e">
+        <f aca="false">AVERAGE(F25:L25)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">MIN(F26:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">MAX(F26:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="e">
+        <f aca="false">AVERAGE(F26:L26)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="false">MIN(F27:L27)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">MAX(F27:L27)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="e">
+        <f aca="false">AVERAGE(F27:L27)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <f aca="false">MIN(F28:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">MAX(F28:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="e">
+        <f aca="false">AVERAGE(F28:L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <f aca="false">MIN(F29:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">MAX(F29:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="e">
+        <f aca="false">AVERAGE(F29:L29)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="false">MIN(F30:L30)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">MAX(F30:L30)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="e">
+        <f aca="false">AVERAGE(F30:L30)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="false">MIN(F31:L31)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">MAX(F31:L31)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="e">
+        <f aca="false">AVERAGE(F31:L31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <f aca="false">MIN(F34:L34)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">MAX(F34:L34)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="e">
+        <f aca="false">AVERAGE(F34:L34)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <f aca="false">MIN(F35:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">MAX(F35:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="e">
+        <f aca="false">AVERAGE(F35:L35)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <f aca="false">MIN(F36:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">MAX(F36:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="e">
+        <f aca="false">AVERAGE(F36:L36)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <f aca="false">MIN(F37:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">MAX(F37:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="e">
+        <f aca="false">AVERAGE(F37:L37)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <f aca="false">MIN(F38:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">MAX(F38:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="e">
+        <f aca="false">AVERAGE(F38:L38)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <f aca="false">MIN(F39:L39)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">MAX(F39:L39)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="e">
+        <f aca="false">AVERAGE(F39:L39)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <f aca="false">MIN(F40:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">MAX(F40:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="e">
+        <f aca="false">AVERAGE(F40:L40)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <f aca="false">MIN(F41:L41)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">MAX(F41:L41)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="e">
+        <f aca="false">AVERAGE(F41:L41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: add 3.5.0 load test results
</commit_message>
<xml_diff>
--- a/load-testing/server/results.xlsx
+++ b/load-testing/server/results.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="3.5.0 vs 3.4.0" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="3.5.0 vs 3.4.0 (Mac M2)" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Server 3.3.0" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Server 3.4.0" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Server 3.4.0 (Mac M2)" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Server 3.5.0-alpha (Mac M2)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Server 3.5.0" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="29">
   <si>
     <t xml:space="preserve">Sequential Ingest Speed Test</t>
   </si>
@@ -112,37 +113,6 @@
   <si>
     <t xml:space="preserve">Run 7</t>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Parallel </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Fragmentation</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Speed Test</t>
-    </r>
-  </si>
 </sst>
 </file>
 
@@ -155,7 +125,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,12 +153,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -287,11 +251,11 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
@@ -706,7 +670,7 @@
       <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
@@ -1203,7 +1167,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
@@ -1610,7 +1574,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
@@ -2008,7 +1972,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
@@ -2412,10 +2376,10 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+      <selection pane="topLeft" activeCell="N35" activeCellId="0" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
@@ -3174,7 +3138,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
@@ -3686,8 +3650,8 @@
         <v>2799</v>
       </c>
       <c r="N34" s="6" t="n">
-        <f aca="false">1-C34/$C$35</f>
-        <v>0.366064648198897</v>
+        <f aca="false">(C34-$C$36)/$C$36</f>
+        <v>-0.3574942274872</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,7 +3691,10 @@
       <c r="L35" s="0" t="n">
         <v>4247</v>
       </c>
-      <c r="N35" s="6"/>
+      <c r="N35" s="6" t="n">
+        <f aca="false">(C35-$C$36)/$C$36</f>
+        <v>0.0135193922966234</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -3766,10 +3733,7 @@
       <c r="L36" s="0" t="n">
         <v>4344</v>
       </c>
-      <c r="N36" s="6" t="n">
-        <f aca="false">1-C36/$C$35</f>
-        <v>0.0133390563608148</v>
-      </c>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -3809,8 +3773,8 @@
         <v>4266</v>
       </c>
       <c r="N37" s="6" t="n">
-        <f aca="false">1-C37/$C$35</f>
-        <v>0.0288242480272063</v>
+        <f aca="false">(C37-$C$36)/$C$36</f>
+        <v>-0.0156945420473179</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,8 +3815,8 @@
         <v>4025</v>
       </c>
       <c r="N38" s="6" t="n">
-        <f aca="false">1-C38/$C$35</f>
-        <v>0.0594644566975929</v>
+        <f aca="false">(C38-$C$36)/$C$36</f>
+        <v>-0.0467489877187698</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,8 +3857,8 @@
         <v>3615</v>
       </c>
       <c r="N39" s="6" t="n">
-        <f aca="false">1-C39/$C$35</f>
-        <v>0.154818899197676</v>
+        <f aca="false">(C39-$C$36)/$C$36</f>
+        <v>-0.143392564334237</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,8 +3899,8 @@
         <v>3458</v>
       </c>
       <c r="N40" s="6" t="n">
-        <f aca="false">1-C40/$C$35</f>
-        <v>0.192722950440783</v>
+        <f aca="false">(C40-$C$36)/$C$36</f>
+        <v>-0.181809055315731</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3977,8 +3941,8 @@
         <v>3345</v>
       </c>
       <c r="N41" s="6" t="n">
-        <f aca="false">1-C41/$C$35</f>
-        <v>0.238154983986529</v>
+        <f aca="false">(C41-$C$36)/$C$36</f>
+        <v>-0.227855302345815</v>
       </c>
     </row>
   </sheetData>
@@ -4000,10 +3964,10 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
@@ -5282,8 +5246,8 @@
         <v>2294</v>
       </c>
       <c r="N34" s="6" t="n">
-        <f aca="false">1-C34/$C$35</f>
-        <v>0.265183797705455</v>
+        <f aca="false">(C34-$C$36)/$C$36</f>
+        <v>-0.265355805243446</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5323,7 +5287,10 @@
       <c r="L35" s="0" t="n">
         <v>3067</v>
       </c>
-      <c r="N35" s="6"/>
+      <c r="N35" s="6" t="n">
+        <f aca="false">(C35-$C$36)/$C$36</f>
+        <v>-0.000234082397003767</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -5362,10 +5329,7 @@
       <c r="L36" s="0" t="n">
         <v>2949</v>
       </c>
-      <c r="N36" s="6" t="n">
-        <f aca="false">1-C36/$C$35</f>
-        <v>-0.000234137204401907</v>
-      </c>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -5405,8 +5369,8 @@
         <v>2946</v>
       </c>
       <c r="N37" s="6" t="n">
-        <f aca="false">1-C37/$C$35</f>
-        <v>0.0217279325684852</v>
+        <f aca="false">(C37-$C$36)/$C$36</f>
+        <v>-0.0219569288389513</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5447,8 +5411,8 @@
         <v>2756</v>
       </c>
       <c r="N38" s="6" t="n">
-        <f aca="false">1-C38/$C$35</f>
-        <v>0.0676188246312339</v>
+        <f aca="false">(C38-$C$36)/$C$36</f>
+        <v>-0.0678370786516854</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,8 +5453,8 @@
         <v>2530</v>
       </c>
       <c r="N39" s="6" t="n">
-        <f aca="false">1-C39/$C$35</f>
-        <v>0.180472957152892</v>
+        <f aca="false">(C39-$C$36)/$C$36</f>
+        <v>-0.180664794007491</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5531,8 +5495,8 @@
         <v>2485</v>
       </c>
       <c r="N40" s="6" t="n">
-        <f aca="false">1-C40/$C$35</f>
-        <v>0.190213064856006</v>
+        <f aca="false">(C40-$C$36)/$C$36</f>
+        <v>-0.190402621722846</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5573,8 +5537,1604 @@
         <v>2407</v>
       </c>
       <c r="N41" s="6" t="n">
-        <f aca="false">1-C41/$C$35</f>
-        <v>0.231421212830719</v>
+        <f aca="false">(C41-$C$36)/$C$36</f>
+        <v>-0.231601123595506</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O41"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <f aca="false">AVERAGE(F2:L2)</f>
+        <v>882.857142857143</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">MIN(F2:L2)</f>
+        <v>749</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">MAX(F2:L2)</f>
+        <v>915</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>749</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>908</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>915</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>909</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>892</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <f aca="false">AVERAGE(F3:L3)</f>
+        <v>1525.42857142857</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">MIN(F3:L3)</f>
+        <v>1410</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">MAX(F3:L3)</f>
+        <v>1577</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1410</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1536</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1543</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1577</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1526</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1543</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1543</v>
+      </c>
+      <c r="N3" s="6" t="n">
+        <f aca="false">(C3-C2)/C2</f>
+        <v>0.727831715210356</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <f aca="false">AVERAGE(F4:L4)</f>
+        <v>1919.14285714286</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">MIN(F4:L4)</f>
+        <v>1814</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">MAX(F4:L4)</f>
+        <v>2016</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1920</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1845</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1934</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1814</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1889</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <f aca="false">(C4-C2)/C2</f>
+        <v>1.17378640776699</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">AVERAGE(F7:L7)</f>
+        <v>329.142857142857</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">MIN(F7:L7)</f>
+        <v>319</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">MAX(F7:L7)</f>
+        <v>338</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <f aca="false">AVERAGE(F8:L8)</f>
+        <v>308.571428571429</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">MIN(F8:L8)</f>
+        <v>304</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">MAX(F8:L8)</f>
+        <v>313</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="N8" s="6" t="n">
+        <f aca="false">(2*C8-C7)/C7</f>
+        <v>0.875</v>
+      </c>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <f aca="false">AVERAGE(F9:L9)</f>
+        <v>259.571428571429</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">MIN(F9:L9)</f>
+        <v>257</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">MAX(F9:L9)</f>
+        <v>263</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <f aca="false">(4*C9-C7)/C7</f>
+        <v>2.15451388888889</v>
+      </c>
+      <c r="O9" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <f aca="false">AVERAGE(F12:L12)</f>
+        <v>834.857142857143</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">MIN(F12:L12)</f>
+        <v>824</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">MAX(F12:L12)</f>
+        <v>841</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>829</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>841</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>824</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>834</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>837</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>839</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="N12" s="6" t="n">
+        <f aca="false">(C12-$C$2)/$C$2</f>
+        <v>-0.054368932038835</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <f aca="false">AVERAGE(F13:L13)</f>
+        <v>1450.71428571429</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">MIN(F13:L13)</f>
+        <v>1418</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">MAX(F13:L13)</f>
+        <v>1466</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1466</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1455</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1466</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1418</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1441</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1447</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1462</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <f aca="false">(C13-$C$3)/$C$3</f>
+        <v>-0.0489792095898107</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <f aca="false">AVERAGE(F14:L14)</f>
+        <v>1932.57142857143</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">MIN(F14:L14)</f>
+        <v>1890</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <f aca="false">MAX(F14:L14)</f>
+        <v>1980</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1965</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1939</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1908</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1980</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1919</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>1890</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>1927</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <f aca="false">(C14-$C$4)/$C$4</f>
+        <v>0.0069971713562603</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <f aca="false">AVERAGE(F15:L15)</f>
+        <v>774.857142857143</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">MIN(F15:L15)</f>
+        <v>750</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <f aca="false">MAX(F15:L15)</f>
+        <v>784</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>783</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>781</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>784</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>770</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>781</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>775</v>
+      </c>
+      <c r="N15" s="6" t="n">
+        <f aca="false">(C15-$C$2)/$C$2</f>
+        <v>-0.122330097087379</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <f aca="false">AVERAGE(F16:L16)</f>
+        <v>1362.71428571429</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">MIN(F16:L16)</f>
+        <v>1335</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <f aca="false">MAX(F16:L16)</f>
+        <v>1398</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1391</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1353</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1362</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1355</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1335</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>1398</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>1345</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <f aca="false">(C16-$C$3)/$C$3</f>
+        <v>-0.106667915339951</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <f aca="false">AVERAGE(F17:L17)</f>
+        <v>1891.28571428571</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">MIN(F17:L17)</f>
+        <v>1815</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">MAX(F17:L17)</f>
+        <v>1987</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1876</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1854</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1905</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1905</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1987</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>1815</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>1897</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <f aca="false">(C17-$C$4)/$C$4</f>
+        <v>-0.0145154086645824</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <f aca="false">AVERAGE(F18:L18)</f>
+        <v>693.142857142857</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">MIN(F18:L18)</f>
+        <v>674</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">MAX(F18:L18)</f>
+        <v>706</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>699</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>696</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>674</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>706</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>691</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <f aca="false">(C18-$C$2)/$C$2</f>
+        <v>-0.214886731391586</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <f aca="false">AVERAGE(F19:L19)</f>
+        <v>1228.85714285714</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">MIN(F19:L19)</f>
+        <v>1212</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">MAX(F19:L19)</f>
+        <v>1239</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1227</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1237</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1212</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1239</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1228</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1231</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>1228</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <f aca="false">(C19-$C$3)/$C$3</f>
+        <v>-0.194418430417681</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <f aca="false">AVERAGE(F20:L20)</f>
+        <v>1779.42857142857</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">MIN(F20:L20)</f>
+        <v>1737</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">MAX(F20:L20)</f>
+        <v>1808</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1789</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1782</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1770</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1801</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>1808</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>1769</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>1737</v>
+      </c>
+      <c r="N20" s="6" t="n">
+        <f aca="false">(C20-$C$4)/$C$4</f>
+        <v>-0.0728003573023672</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <f aca="false">AVERAGE(F23:L23)</f>
+        <v>316.142857142857</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">MIN(F23:L23)</f>
+        <v>312</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">MAX(F23:L23)</f>
+        <v>320</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="N23" s="6" t="n">
+        <f aca="false">(C23-$C$7)/$C$7</f>
+        <v>-0.0394965277777778</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <f aca="false">AVERAGE(F24:L24)</f>
+        <v>287.571428571429</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">MIN(F24:L24)</f>
+        <v>284</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">MAX(F24:L24)</f>
+        <v>291</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>285</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>284</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>285</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="N24" s="6" t="n">
+        <f aca="false">(C24-$C$8)/$C$8</f>
+        <v>-0.0680555555555556</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <f aca="false">AVERAGE(F25:L25)</f>
+        <v>240.142857142857</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">MIN(F25:L25)</f>
+        <v>238</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">MAX(F25:L25)</f>
+        <v>243</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="N25" s="6" t="n">
+        <f aca="false">(C25-$C$9)/$C$9</f>
+        <v>-0.0748486516235553</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <f aca="false">AVERAGE(F26:L26)</f>
+        <v>314.285714285714</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">MIN(F26:L26)</f>
+        <v>311</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <f aca="false">MAX(F26:L26)</f>
+        <v>319</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="N26" s="6" t="n">
+        <f aca="false">(C26-$C$7)/$C$7</f>
+        <v>-0.045138888888889</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <f aca="false">AVERAGE(F27:L27)</f>
+        <v>288.571428571429</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">MIN(F27:L27)</f>
+        <v>286</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <f aca="false">MAX(F27:L27)</f>
+        <v>292</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>289</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>292</v>
+      </c>
+      <c r="N27" s="6" t="n">
+        <f aca="false">(C27-$C$8)/$C$8</f>
+        <v>-0.0648148148148148</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <f aca="false">AVERAGE(F28:L28)</f>
+        <v>242.285714285714</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">MIN(F28:L28)</f>
+        <v>240</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <f aca="false">MAX(F28:L28)</f>
+        <v>245</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>244</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="N28" s="6" t="n">
+        <f aca="false">(C28-$C$9)/$C$9</f>
+        <v>-0.0665932856356632</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <f aca="false">AVERAGE(F29:L29)</f>
+        <v>311.714285714286</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">MIN(F29:L29)</f>
+        <v>308</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <f aca="false">MAX(F29:L29)</f>
+        <v>315</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="N29" s="6" t="n">
+        <f aca="false">(C29-$C$7)/$C$7</f>
+        <v>-0.0529513888888889</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5" t="n">
+        <f aca="false">AVERAGE(F30:L30)</f>
+        <v>286.428571428571</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">MIN(F30:L30)</f>
+        <v>278</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">MAX(F30:L30)</f>
+        <v>294</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>281</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>278</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>284</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>289</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>292</v>
+      </c>
+      <c r="N30" s="6" t="n">
+        <f aca="false">(C30-$C$8)/$C$8</f>
+        <v>-0.0717592592592592</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="5" t="n">
+        <f aca="false">AVERAGE(F31:L31)</f>
+        <v>240.714285714286</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">MIN(F31:L31)</f>
+        <v>239</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">MAX(F31:L31)</f>
+        <v>243</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="N31" s="6" t="n">
+        <f aca="false">(C31-$C$9)/$C$9</f>
+        <v>-0.0726472206934507</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <f aca="false">AVERAGE(F34:L34)</f>
+        <v>698</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">MIN(F34:L34)</f>
+        <v>683</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <f aca="false">MAX(F34:L34)</f>
+        <v>716</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>683</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>706</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>685</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>716</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>707</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>696</v>
+      </c>
+      <c r="N34" s="6" t="n">
+        <f aca="false">(C34-$C$36)/$C$36</f>
+        <v>-0.513346613545817</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="5" t="n">
+        <f aca="false">AVERAGE(F35:L35)</f>
+        <v>1342.28571428571</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">MIN(F35:L35)</f>
+        <v>1272</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">MAX(F35:L35)</f>
+        <v>1372</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1336</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>1358</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1334</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>1361</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>1372</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>1363</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>1272</v>
+      </c>
+      <c r="N35" s="6" t="n">
+        <f aca="false">(C35-$C$36)/$C$36</f>
+        <v>-0.0641434262948207</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <f aca="false">AVERAGE(F36:L36)</f>
+        <v>1434.28571428571</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">MIN(F36:L36)</f>
+        <v>1402</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">MAX(F36:L36)</f>
+        <v>1473</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1402</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>1427</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>1423</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>1441</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>1473</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>1448</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>1426</v>
+      </c>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <f aca="false">AVERAGE(F37:L37)</f>
+        <v>1375.28571428571</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">MIN(F37:L37)</f>
+        <v>1319</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <f aca="false">MAX(F37:L37)</f>
+        <v>1434</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1324</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>1319</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>1377</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>1394</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>1432</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>1434</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>1347</v>
+      </c>
+      <c r="N37" s="6" t="n">
+        <f aca="false">(C37-$C$36)/$C$36</f>
+        <v>-0.0411354581673307</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="5" t="n">
+        <f aca="false">AVERAGE(F38:L38)</f>
+        <v>1251.71428571429</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">MIN(F38:L38)</f>
+        <v>1235</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <f aca="false">MAX(F38:L38)</f>
+        <v>1279</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1245</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>1239</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>1235</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>1248</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>1279</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>1271</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>1245</v>
+      </c>
+      <c r="N38" s="6" t="n">
+        <f aca="false">(C38-$C$36)/$C$36</f>
+        <v>-0.127290836653386</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <f aca="false">AVERAGE(F39:L39)</f>
+        <v>1178.71428571429</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">MIN(F39:L39)</f>
+        <v>1148</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">MAX(F39:L39)</f>
+        <v>1210</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>1148</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>1194</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1152</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>1210</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>1170</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>1199</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>1178</v>
+      </c>
+      <c r="N39" s="6" t="n">
+        <f aca="false">(C39-$C$36)/$C$36</f>
+        <v>-0.178187250996016</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <f aca="false">AVERAGE(F40:L40)</f>
+        <v>1024</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">MIN(F40:L40)</f>
+        <v>991</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">MAX(F40:L40)</f>
+        <v>1055</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1005</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1033</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>991</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>1055</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>1050</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>1007</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>1027</v>
+      </c>
+      <c r="N40" s="6" t="n">
+        <f aca="false">(C40-$C$36)/$C$36</f>
+        <v>-0.28605577689243</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="5" t="n">
+        <f aca="false">AVERAGE(F41:L41)</f>
+        <v>1120.85714285714</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">MIN(F41:L41)</f>
+        <v>1081</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <f aca="false">MAX(F41:L41)</f>
+        <v>1152</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>1081</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>1105</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>1116</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>1152</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>1136</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>1121</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>1135</v>
+      </c>
+      <c r="N41" s="6" t="n">
+        <f aca="false">(C41-$C$36)/$C$36</f>
+        <v>-0.218525896414343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>